<commit_message>
1 - Class Time per Occupation Calculation 2 - Total Screen Time Calculation (WD,WY) 3 - Occupations Type [occ1,occ2,occ3]  A. (1 = Student, 2 = Work, 3 = Volunteer) 4. Total Travel Time Calculation 5. Total Day Travel Calculation  A. TF = Days , Time  B. AP = Days , Time  C. AF = (Days*Time)
</commit_message>
<xml_diff>
--- a/SSHRCData.xlsx
+++ b/SSHRCData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jglts\Repos\SB-SWB Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12836ADC-B20A-4820-AC77-C4526AA17FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6498A09C-4932-45B0-8787-F957EEB43CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-5290" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2467,8 +2467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:PT47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" topLeftCell="CX1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="DE14" sqref="DE14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>